<commit_message>
start util for handling 2D table of excel
</commit_message>
<xml_diff>
--- a/src/test/resources/2007_1.xlsx
+++ b/src/test/resources/2007_1.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="12832" windowHeight="7800" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12828" windowHeight="7800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1318" uniqueCount="671">
   <si>
     <t>表头1</t>
   </si>
@@ -2032,368 +2032,31 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="_ \￥* #,##0_ ;_ \￥* \-#,##0_ ;_ \￥* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ \￥* #,##0.00_ ;_ \￥* \-#,##0.00_ ;_ \￥* &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="21">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <sz val="9"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -2401,313 +2064,27 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
+  </cellStyleXfs>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-  </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="49">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+  <cellStyles count="1">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -3033,35 +2410,36 @@
       </a:style>
     </a:lnDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L222"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="9" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="12.3984375" customWidth="1"/>
+    <col min="5" max="5" width="7.3984375" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="12.5" customWidth="1"/>
     <col min="8" max="8" width="9" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2" t="s">
+      <c r="E2" s="1"/>
+      <c r="F2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="G2" t="s">
@@ -3070,58 +2448,58 @@
       <c r="H2" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-    </row>
-    <row r="3" spans="2:12">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="4"/>
       <c r="G3" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2" t="s">
+      <c r="J3" s="4"/>
+      <c r="K3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="2"/>
-    </row>
-    <row r="4" spans="2:12">
+      <c r="L3" s="4"/>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="4"/>
       <c r="G4" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="2:12">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>16</v>
       </c>
@@ -3153,7 +2531,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" hidden="1" spans="2:12">
+    <row r="6" spans="2:12" ht="18.600000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>22</v>
       </c>
@@ -3182,7 +2560,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:12">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>23</v>
       </c>
@@ -3214,7 +2592,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="2:12">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>27</v>
       </c>
@@ -3243,7 +2621,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="2:12">
+    <row r="9" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>19</v>
       </c>
@@ -3272,7 +2650,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="2:12">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>32</v>
       </c>
@@ -3301,7 +2679,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="2:12">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>35</v>
       </c>
@@ -3330,7 +2708,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="2:12">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>38</v>
       </c>
@@ -3359,7 +2737,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="2:12">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>41</v>
       </c>
@@ -3388,7 +2766,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="2:12">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>44</v>
       </c>
@@ -3417,7 +2795,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="2:12">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>47</v>
       </c>
@@ -3446,7 +2824,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="2:12">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>50</v>
       </c>
@@ -3475,7 +2853,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="2:12">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>53</v>
       </c>
@@ -3504,7 +2882,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="2:12">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>56</v>
       </c>
@@ -3533,7 +2911,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="2:12">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>59</v>
       </c>
@@ -3562,7 +2940,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="2:12">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>62</v>
       </c>
@@ -3591,7 +2969,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="2:12">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>65</v>
       </c>
@@ -3620,7 +2998,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="2:12">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>68</v>
       </c>
@@ -3649,7 +3027,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="2:12">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>71</v>
       </c>
@@ -3678,7 +3056,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="2:12">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>74</v>
       </c>
@@ -3707,7 +3085,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="2:12">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>77</v>
       </c>
@@ -3736,7 +3114,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="2:12">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>80</v>
       </c>
@@ -3765,7 +3143,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="2:12">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>83</v>
       </c>
@@ -3794,7 +3172,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="2:12">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>86</v>
       </c>
@@ -3823,7 +3201,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="2:12">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>89</v>
       </c>
@@ -3852,7 +3230,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="2:12">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>92</v>
       </c>
@@ -3881,7 +3259,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="2:12">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>95</v>
       </c>
@@ -3910,7 +3288,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="2:12">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>98</v>
       </c>
@@ -3939,7 +3317,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="2:12">
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>101</v>
       </c>
@@ -3968,7 +3346,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="2:12">
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>104</v>
       </c>
@@ -3997,7 +3375,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="2:12">
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>107</v>
       </c>
@@ -4026,7 +3404,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="2:12">
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>110</v>
       </c>
@@ -4055,7 +3433,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="2:12">
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>113</v>
       </c>
@@ -4084,7 +3462,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="2:12">
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>116</v>
       </c>
@@ -4113,7 +3491,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="2:12">
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>119</v>
       </c>
@@ -4142,7 +3520,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="2:12">
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>122</v>
       </c>
@@ -4171,7 +3549,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="2:12">
+    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>125</v>
       </c>
@@ -4200,7 +3578,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="2:12">
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>128</v>
       </c>
@@ -4229,7 +3607,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="2:12">
+    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>131</v>
       </c>
@@ -4258,7 +3636,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="2:12">
+    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>134</v>
       </c>
@@ -4287,7 +3665,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="2:12">
+    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>137</v>
       </c>
@@ -4316,7 +3694,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="2:12">
+    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>140</v>
       </c>
@@ -4345,7 +3723,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="2:12">
+    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>143</v>
       </c>
@@ -4374,7 +3752,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="2:12">
+    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>146</v>
       </c>
@@ -4403,7 +3781,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="49" spans="2:12">
+    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>149</v>
       </c>
@@ -4432,7 +3810,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="50" spans="2:12">
+    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>152</v>
       </c>
@@ -4461,7 +3839,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="2:12">
+    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>155</v>
       </c>
@@ -4490,7 +3868,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="52" spans="2:12">
+    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>158</v>
       </c>
@@ -4519,7 +3897,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="53" spans="2:12">
+    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>161</v>
       </c>
@@ -4548,7 +3926,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="2:12">
+    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>164</v>
       </c>
@@ -4577,7 +3955,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="2:12">
+    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>167</v>
       </c>
@@ -4606,7 +3984,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="56" spans="2:12">
+    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>170</v>
       </c>
@@ -4635,7 +4013,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="57" spans="2:12">
+    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>173</v>
       </c>
@@ -4664,7 +4042,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="58" spans="2:12">
+    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>176</v>
       </c>
@@ -4693,7 +4071,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="59" spans="2:12">
+    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>179</v>
       </c>
@@ -4722,7 +4100,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="60" spans="2:12">
+    <row r="60" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>182</v>
       </c>
@@ -4751,7 +4129,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="61" spans="2:12">
+    <row r="61" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>185</v>
       </c>
@@ -4780,7 +4158,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="62" spans="2:12">
+    <row r="62" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>188</v>
       </c>
@@ -4809,7 +4187,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="63" spans="2:12">
+    <row r="63" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>191</v>
       </c>
@@ -4838,7 +4216,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="64" spans="2:12">
+    <row r="64" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>194</v>
       </c>
@@ -4867,7 +4245,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="65" spans="2:12">
+    <row r="65" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>197</v>
       </c>
@@ -4896,7 +4274,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="66" spans="2:12">
+    <row r="66" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>200</v>
       </c>
@@ -4925,7 +4303,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="67" spans="2:12">
+    <row r="67" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>203</v>
       </c>
@@ -4954,7 +4332,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="68" spans="2:12">
+    <row r="68" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>206</v>
       </c>
@@ -4983,7 +4361,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="69" spans="2:12">
+    <row r="69" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>209</v>
       </c>
@@ -5012,7 +4390,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="70" spans="2:12">
+    <row r="70" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>212</v>
       </c>
@@ -5041,7 +4419,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="71" spans="2:12">
+    <row r="71" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>215</v>
       </c>
@@ -5070,7 +4448,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="72" spans="2:12">
+    <row r="72" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>218</v>
       </c>
@@ -5099,7 +4477,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="73" spans="2:12">
+    <row r="73" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>221</v>
       </c>
@@ -5128,7 +4506,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="74" spans="2:12">
+    <row r="74" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>224</v>
       </c>
@@ -5157,7 +4535,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="75" spans="2:12">
+    <row r="75" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>227</v>
       </c>
@@ -5186,7 +4564,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="76" spans="2:12">
+    <row r="76" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>230</v>
       </c>
@@ -5215,7 +4593,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="77" spans="2:12">
+    <row r="77" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>233</v>
       </c>
@@ -5244,7 +4622,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="78" spans="2:12">
+    <row r="78" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>236</v>
       </c>
@@ -5273,7 +4651,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="79" spans="2:12">
+    <row r="79" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>239</v>
       </c>
@@ -5302,7 +4680,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="80" spans="2:12">
+    <row r="80" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>242</v>
       </c>
@@ -5331,7 +4709,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="81" spans="2:12">
+    <row r="81" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>245</v>
       </c>
@@ -5360,7 +4738,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="82" spans="2:12">
+    <row r="82" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>248</v>
       </c>
@@ -5389,7 +4767,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="83" spans="2:12">
+    <row r="83" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>251</v>
       </c>
@@ -5418,7 +4796,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="84" spans="2:12">
+    <row r="84" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>254</v>
       </c>
@@ -5447,7 +4825,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="85" spans="2:12">
+    <row r="85" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>257</v>
       </c>
@@ -5476,7 +4854,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="86" spans="2:12">
+    <row r="86" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>260</v>
       </c>
@@ -5505,7 +4883,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="87" spans="2:12">
+    <row r="87" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>263</v>
       </c>
@@ -5534,7 +4912,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="88" spans="2:12">
+    <row r="88" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>266</v>
       </c>
@@ -5563,7 +4941,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="89" spans="2:12">
+    <row r="89" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>269</v>
       </c>
@@ -5592,7 +4970,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="90" spans="2:12">
+    <row r="90" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>272</v>
       </c>
@@ -5621,7 +4999,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="91" spans="2:12">
+    <row r="91" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>275</v>
       </c>
@@ -5650,7 +5028,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="92" spans="2:12">
+    <row r="92" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>278</v>
       </c>
@@ -5679,7 +5057,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="93" spans="2:12">
+    <row r="93" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>281</v>
       </c>
@@ -5708,7 +5086,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="94" spans="2:12">
+    <row r="94" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>284</v>
       </c>
@@ -5737,7 +5115,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="95" spans="2:12">
+    <row r="95" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>287</v>
       </c>
@@ -5766,7 +5144,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="96" spans="2:12">
+    <row r="96" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>290</v>
       </c>
@@ -5795,7 +5173,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="97" spans="2:12">
+    <row r="97" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
         <v>293</v>
       </c>
@@ -5824,7 +5202,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="98" spans="2:12">
+    <row r="98" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>296</v>
       </c>
@@ -5853,7 +5231,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="99" spans="2:12">
+    <row r="99" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
         <v>299</v>
       </c>
@@ -5882,7 +5260,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="100" spans="2:12">
+    <row r="100" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>302</v>
       </c>
@@ -5911,7 +5289,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="101" spans="2:12">
+    <row r="101" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>305</v>
       </c>
@@ -5940,7 +5318,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="102" spans="2:12">
+    <row r="102" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>308</v>
       </c>
@@ -5969,7 +5347,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="103" spans="2:12">
+    <row r="103" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>311</v>
       </c>
@@ -5998,7 +5376,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="104" spans="2:12">
+    <row r="104" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
         <v>314</v>
       </c>
@@ -6027,7 +5405,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="105" spans="2:12">
+    <row r="105" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
         <v>317</v>
       </c>
@@ -6056,7 +5434,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="106" spans="2:12">
+    <row r="106" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
         <v>320</v>
       </c>
@@ -6085,7 +5463,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="107" spans="2:12">
+    <row r="107" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
         <v>323</v>
       </c>
@@ -6114,7 +5492,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="108" spans="2:12">
+    <row r="108" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>326</v>
       </c>
@@ -6143,7 +5521,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="109" spans="2:12">
+    <row r="109" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
         <v>329</v>
       </c>
@@ -6172,7 +5550,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="110" spans="2:12">
+    <row r="110" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
         <v>332</v>
       </c>
@@ -6201,7 +5579,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="111" spans="2:12">
+    <row r="111" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
         <v>335</v>
       </c>
@@ -6230,7 +5608,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="112" spans="2:12">
+    <row r="112" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
         <v>338</v>
       </c>
@@ -6259,7 +5637,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="113" spans="2:12">
+    <row r="113" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
         <v>341</v>
       </c>
@@ -6288,7 +5666,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="114" spans="2:12">
+    <row r="114" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
         <v>344</v>
       </c>
@@ -6317,7 +5695,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="115" spans="2:12">
+    <row r="115" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
         <v>347</v>
       </c>
@@ -6346,7 +5724,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="116" spans="2:12">
+    <row r="116" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
         <v>350</v>
       </c>
@@ -6375,7 +5753,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="117" spans="2:12">
+    <row r="117" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
         <v>353</v>
       </c>
@@ -6404,7 +5782,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="118" spans="2:12">
+    <row r="118" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
         <v>356</v>
       </c>
@@ -6433,7 +5811,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="119" spans="2:12">
+    <row r="119" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
         <v>359</v>
       </c>
@@ -6462,7 +5840,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="120" spans="2:12">
+    <row r="120" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
         <v>362</v>
       </c>
@@ -6491,7 +5869,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="121" spans="2:12">
+    <row r="121" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
         <v>365</v>
       </c>
@@ -6520,7 +5898,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="122" spans="2:12">
+    <row r="122" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
         <v>368</v>
       </c>
@@ -6549,7 +5927,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="123" spans="2:12">
+    <row r="123" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
         <v>371</v>
       </c>
@@ -6578,7 +5956,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="124" spans="2:12">
+    <row r="124" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
         <v>374</v>
       </c>
@@ -6607,7 +5985,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="125" spans="2:12">
+    <row r="125" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
         <v>377</v>
       </c>
@@ -6636,7 +6014,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="126" spans="2:12">
+    <row r="126" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
         <v>380</v>
       </c>
@@ -6665,7 +6043,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="127" spans="2:12">
+    <row r="127" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
         <v>383</v>
       </c>
@@ -6694,7 +6072,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="128" spans="2:12">
+    <row r="128" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
         <v>386</v>
       </c>
@@ -6723,7 +6101,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="129" spans="2:12">
+    <row r="129" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
         <v>389</v>
       </c>
@@ -6752,7 +6130,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="130" spans="2:12">
+    <row r="130" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
         <v>392</v>
       </c>
@@ -6781,7 +6159,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="131" spans="2:12">
+    <row r="131" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
         <v>395</v>
       </c>
@@ -6810,7 +6188,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="132" spans="2:12">
+    <row r="132" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
         <v>398</v>
       </c>
@@ -6839,7 +6217,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="133" spans="2:12">
+    <row r="133" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
         <v>401</v>
       </c>
@@ -6868,7 +6246,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="134" spans="2:12">
+    <row r="134" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
         <v>404</v>
       </c>
@@ -6897,7 +6275,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="135" spans="2:12">
+    <row r="135" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
         <v>407</v>
       </c>
@@ -6926,7 +6304,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="136" spans="2:12">
+    <row r="136" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
         <v>410</v>
       </c>
@@ -6955,7 +6333,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="137" spans="2:12">
+    <row r="137" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
         <v>413</v>
       </c>
@@ -6984,7 +6362,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="138" spans="2:12">
+    <row r="138" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
         <v>416</v>
       </c>
@@ -7013,7 +6391,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="139" spans="2:12">
+    <row r="139" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
         <v>419</v>
       </c>
@@ -7042,7 +6420,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="140" spans="2:12">
+    <row r="140" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
         <v>422</v>
       </c>
@@ -7071,7 +6449,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="141" spans="2:12">
+    <row r="141" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
         <v>425</v>
       </c>
@@ -7100,7 +6478,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="142" spans="2:12">
+    <row r="142" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
         <v>428</v>
       </c>
@@ -7129,7 +6507,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="143" spans="2:12">
+    <row r="143" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
         <v>431</v>
       </c>
@@ -7158,7 +6536,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="144" spans="2:12">
+    <row r="144" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
         <v>434</v>
       </c>
@@ -7187,7 +6565,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="145" spans="2:12">
+    <row r="145" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
         <v>437</v>
       </c>
@@ -7216,7 +6594,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="146" spans="2:12">
+    <row r="146" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
         <v>440</v>
       </c>
@@ -7245,7 +6623,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="147" spans="2:12">
+    <row r="147" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
         <v>443</v>
       </c>
@@ -7274,7 +6652,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="148" spans="2:12">
+    <row r="148" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
         <v>446</v>
       </c>
@@ -7303,7 +6681,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="149" spans="2:12">
+    <row r="149" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
         <v>449</v>
       </c>
@@ -7332,7 +6710,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="150" spans="2:12">
+    <row r="150" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
         <v>452</v>
       </c>
@@ -7361,7 +6739,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="151" spans="2:12">
+    <row r="151" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
         <v>455</v>
       </c>
@@ -7390,7 +6768,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="152" spans="2:12">
+    <row r="152" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
         <v>458</v>
       </c>
@@ -7419,7 +6797,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="153" spans="2:12">
+    <row r="153" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
         <v>461</v>
       </c>
@@ -7448,7 +6826,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="154" spans="2:12">
+    <row r="154" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
         <v>464</v>
       </c>
@@ -7477,7 +6855,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="155" spans="2:12">
+    <row r="155" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
         <v>467</v>
       </c>
@@ -7506,7 +6884,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="156" spans="2:12">
+    <row r="156" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
         <v>470</v>
       </c>
@@ -7535,7 +6913,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="157" spans="2:12">
+    <row r="157" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
         <v>473</v>
       </c>
@@ -7564,7 +6942,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="158" spans="2:12">
+    <row r="158" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
         <v>476</v>
       </c>
@@ -7593,7 +6971,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="159" spans="2:12">
+    <row r="159" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
         <v>479</v>
       </c>
@@ -7622,7 +7000,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="160" spans="2:12">
+    <row r="160" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
         <v>482</v>
       </c>
@@ -7651,7 +7029,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="161" spans="2:12">
+    <row r="161" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
         <v>485</v>
       </c>
@@ -7680,7 +7058,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="162" spans="2:12">
+    <row r="162" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
         <v>488</v>
       </c>
@@ -7709,7 +7087,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="163" spans="2:12">
+    <row r="163" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B163" t="s">
         <v>491</v>
       </c>
@@ -7738,7 +7116,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="164" spans="2:12">
+    <row r="164" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
         <v>494</v>
       </c>
@@ -7767,7 +7145,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="165" spans="2:12">
+    <row r="165" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
         <v>497</v>
       </c>
@@ -7796,7 +7174,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="166" spans="2:12">
+    <row r="166" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
         <v>500</v>
       </c>
@@ -7825,7 +7203,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="167" spans="2:12">
+    <row r="167" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
         <v>503</v>
       </c>
@@ -7854,7 +7232,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="168" spans="2:12">
+    <row r="168" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
         <v>506</v>
       </c>
@@ -7883,7 +7261,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="169" spans="2:12">
+    <row r="169" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
         <v>509</v>
       </c>
@@ -7912,7 +7290,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="170" spans="2:12">
+    <row r="170" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
         <v>512</v>
       </c>
@@ -7941,7 +7319,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="171" spans="2:12">
+    <row r="171" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B171" t="s">
         <v>515</v>
       </c>
@@ -7970,7 +7348,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="172" spans="2:12">
+    <row r="172" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
         <v>518</v>
       </c>
@@ -7999,7 +7377,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="173" spans="2:12">
+    <row r="173" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
         <v>521</v>
       </c>
@@ -8028,7 +7406,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="174" spans="2:12">
+    <row r="174" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B174" t="s">
         <v>524</v>
       </c>
@@ -8057,7 +7435,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="175" spans="2:12">
+    <row r="175" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B175" t="s">
         <v>527</v>
       </c>
@@ -8086,7 +7464,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="176" spans="2:12">
+    <row r="176" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B176" t="s">
         <v>530</v>
       </c>
@@ -8115,7 +7493,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="177" spans="2:12">
+    <row r="177" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
         <v>533</v>
       </c>
@@ -8144,7 +7522,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="178" spans="2:12">
+    <row r="178" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B178" t="s">
         <v>536</v>
       </c>
@@ -8173,7 +7551,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="179" spans="2:12">
+    <row r="179" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
         <v>539</v>
       </c>
@@ -8202,7 +7580,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="180" spans="2:12">
+    <row r="180" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B180" t="s">
         <v>542</v>
       </c>
@@ -8231,7 +7609,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="181" spans="2:12">
+    <row r="181" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B181" t="s">
         <v>545</v>
       </c>
@@ -8260,7 +7638,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="182" spans="2:12">
+    <row r="182" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
         <v>548</v>
       </c>
@@ -8289,7 +7667,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="183" spans="2:12">
+    <row r="183" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
         <v>551</v>
       </c>
@@ -8318,7 +7696,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="184" spans="2:12">
+    <row r="184" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B184" t="s">
         <v>554</v>
       </c>
@@ -8347,7 +7725,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="185" spans="2:12">
+    <row r="185" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
         <v>557</v>
       </c>
@@ -8376,7 +7754,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="186" spans="2:12">
+    <row r="186" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
         <v>560</v>
       </c>
@@ -8405,7 +7783,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="187" spans="2:12">
+    <row r="187" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
         <v>563</v>
       </c>
@@ -8434,7 +7812,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="188" spans="2:12">
+    <row r="188" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
         <v>566</v>
       </c>
@@ -8463,7 +7841,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="189" spans="2:12">
+    <row r="189" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
         <v>569</v>
       </c>
@@ -8492,7 +7870,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="190" spans="2:12">
+    <row r="190" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B190" t="s">
         <v>572</v>
       </c>
@@ -8521,7 +7899,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="191" spans="2:12">
+    <row r="191" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B191" t="s">
         <v>575</v>
       </c>
@@ -8550,7 +7928,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="192" spans="2:12">
+    <row r="192" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B192" t="s">
         <v>578</v>
       </c>
@@ -8579,7 +7957,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="193" spans="2:12">
+    <row r="193" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B193" t="s">
         <v>581</v>
       </c>
@@ -8608,7 +7986,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="194" spans="2:12">
+    <row r="194" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B194" t="s">
         <v>584</v>
       </c>
@@ -8637,7 +8015,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="195" spans="2:12">
+    <row r="195" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B195" t="s">
         <v>587</v>
       </c>
@@ -8666,7 +8044,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="196" spans="2:12">
+    <row r="196" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B196" t="s">
         <v>590</v>
       </c>
@@ -8695,7 +8073,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="197" spans="2:12">
+    <row r="197" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B197" t="s">
         <v>593</v>
       </c>
@@ -8724,7 +8102,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="198" spans="2:12">
+    <row r="198" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B198" t="s">
         <v>596</v>
       </c>
@@ -8753,7 +8131,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="199" spans="2:12">
+    <row r="199" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B199" t="s">
         <v>599</v>
       </c>
@@ -8782,7 +8160,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="200" spans="2:12">
+    <row r="200" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B200" t="s">
         <v>602</v>
       </c>
@@ -8811,7 +8189,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="201" spans="2:12">
+    <row r="201" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B201" t="s">
         <v>605</v>
       </c>
@@ -8840,7 +8218,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="202" spans="2:12">
+    <row r="202" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B202" t="s">
         <v>608</v>
       </c>
@@ -8869,7 +8247,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="203" spans="2:12">
+    <row r="203" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B203" t="s">
         <v>611</v>
       </c>
@@ -8898,7 +8276,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="204" spans="2:12">
+    <row r="204" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B204" t="s">
         <v>614</v>
       </c>
@@ -8927,7 +8305,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="205" spans="2:12">
+    <row r="205" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B205" t="s">
         <v>617</v>
       </c>
@@ -8956,7 +8334,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="206" spans="2:12">
+    <row r="206" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B206" t="s">
         <v>620</v>
       </c>
@@ -8985,7 +8363,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="207" spans="2:12">
+    <row r="207" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B207" t="s">
         <v>623</v>
       </c>
@@ -9014,7 +8392,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="208" spans="2:12">
+    <row r="208" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B208" t="s">
         <v>626</v>
       </c>
@@ -9043,7 +8421,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="209" spans="2:12">
+    <row r="209" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B209" t="s">
         <v>629</v>
       </c>
@@ -9072,7 +8450,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="210" spans="2:12">
+    <row r="210" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B210" t="s">
         <v>632</v>
       </c>
@@ -9101,7 +8479,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="211" spans="2:12">
+    <row r="211" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B211" t="s">
         <v>635</v>
       </c>
@@ -9130,7 +8508,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="212" spans="2:12">
+    <row r="212" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B212" t="s">
         <v>638</v>
       </c>
@@ -9159,7 +8537,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="213" spans="2:12">
+    <row r="213" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B213" t="s">
         <v>641</v>
       </c>
@@ -9188,7 +8566,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="214" spans="2:12">
+    <row r="214" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B214" t="s">
         <v>644</v>
       </c>
@@ -9217,7 +8595,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="215" spans="2:12">
+    <row r="215" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B215" t="s">
         <v>647</v>
       </c>
@@ -9246,7 +8624,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="216" spans="2:12">
+    <row r="216" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B216" t="s">
         <v>650</v>
       </c>
@@ -9275,7 +8653,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="217" spans="2:12">
+    <row r="217" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B217" t="s">
         <v>653</v>
       </c>
@@ -9304,7 +8682,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="218" spans="2:12">
+    <row r="218" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B218" t="s">
         <v>656</v>
       </c>
@@ -9330,7 +8708,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="219" spans="2:12">
+    <row r="219" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B219" t="s">
         <v>659</v>
       </c>
@@ -9359,7 +8737,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="220" spans="2:12">
+    <row r="220" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B220" t="s">
         <v>662</v>
       </c>
@@ -9385,7 +8763,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="221" spans="2:12">
+    <row r="221" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B221" t="s">
         <v>665</v>
       </c>
@@ -9414,7 +8792,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="222" spans="2:12">
+    <row r="222" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B222" t="s">
         <v>668</v>
       </c>
@@ -9442,14 +8820,14 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B2:C3"/>
     <mergeCell ref="I2:L2"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="D2:D4"/>
     <mergeCell ref="F2:F4"/>
-    <mergeCell ref="B2:C3"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>